<commit_message>
Updating files from internal Dropbox.
</commit_message>
<xml_diff>
--- a/report/indexwebsite.xlsx
+++ b/report/indexwebsite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="1540" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Page views" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
-  <si>
-    <t>/</t>
-  </si>
   <si>
     <t>/ranking</t>
   </si>
@@ -218,13 +215,16 @@
   <si>
     <t>globalguerrillas.typepad.com</t>
   </si>
+  <si>
+    <t>/ [Front page]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -286,7 +286,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
@@ -374,7 +374,7 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>/</c:v>
+                  <c:v>/ [Front page]</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>/ranking</c:v>
@@ -1076,8 +1076,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H359"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1093,33 +1093,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1">
         <v>34824</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
         <v>10314</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>5636</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
         <v>4424</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>4331</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>3376</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>2414</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>1531</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1">
         <f>85464-SUM(B2:B9)</f>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1">
         <v>1408</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>868</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>843</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>765</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>665</v>
@@ -1471,7 +1471,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>643</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>597</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>579</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19">
         <v>548</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>453</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>427</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>349</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>347</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>322</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>311</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>305</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>285</v>
@@ -1806,10 +1806,10 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -4457,7 +4457,7 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -4473,57 +4473,57 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>43</v>
       </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1">
         <v>9564</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1">
         <v>3410</v>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1">
         <f>1847+1584</f>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
         <v>2022</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1">
         <v>1221</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>902</v>
@@ -4644,7 +4644,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>747</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>643</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17">
         <v>489</v>
@@ -4721,10 +4721,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:6">

</xml_diff>